<commit_message>
Update of the verification plan of the HW loop extension of the core CV32E40P for revision 4.3 of RI5CY User Manual
</commit_message>
<xml_diff>
--- a/verif/CV32E40P/VerificationPlan/xpulp_instruction_extensions/CV32E40P_xpulp-hwloop.xlsx
+++ b/verif/CV32E40P/VerificationPlan/xpulp_instruction_extensions/CV32E40P_xpulp-hwloop.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="43">
   <si>
     <t>Requirement Location</t>
   </si>
@@ -49,14 +49,6 @@
   </si>
   <si>
     <t xml:space="preserve"> -------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------- END -----------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------</t>
-  </si>
-  <si>
-    <t>RI5CY: User Manual, rev. 4.2
-Section 7</t>
-  </si>
-  <si>
-    <t>RI5CY: User Manual, rev. 4.2
-Section 14.2</t>
   </si>
   <si>
     <t>lp.starti</t>
@@ -210,18 +202,7 @@
     <t>CSR mapping</t>
   </si>
   <si>
-    <t>Single loop</t>
-  </si>
-  <si>
-    <t>Nested loops</t>
-  </si>
-  <si>
     <t>Programming rules</t>
-  </si>
-  <si>
-    <t>** HWloop begin address must be ALIGNED
-** No compressed instructions allowed in the HWLoop body
-** [Minimum 3 instructions]</t>
   </si>
   <si>
     <t>Compliance tests: correct test signature.</t>
@@ -276,23 +257,28 @@
 </t>
   </si>
   <si>
-    <t>Support of nested loops with a priority to hardware loop 0.
-- If the two hardware loops have identical end addresses and if the counter of loop 0 is greater than 1, only the counter of loop 0 is decremented and the core jumps to the start of loop 0.
-- If the two hardware loops have identical end addresses and if the counter of loop 0 is equal to 1, the counters of loop 0 and loop 1 are decremented and the core then jumps to the start of loop 1.</t>
-  </si>
-  <si>
-    <t>Compliance tests: correct test signature.
-Random tests: RTL matches ISS.</t>
-  </si>
-  <si>
-    <t>Check that loop 0 has higher priority when the two hardware loops have identical end addresses.
-Exercise with different nested loop sizes (including zero).</t>
-  </si>
-  <si>
     <t>Compliance tests: correct test signature.
 Random tests: RTL matches ISS.
 A backdoor to the PC and to the CSR would be desirable. The extension of the reference ISS with HW loops would be desirable.
 Constraints on the random tests of the HW loop would be desirable to limit simulation time (size of loop body | number of iterations | addresses of loops).</t>
+  </si>
+  <si>
+    <t>** Start address of an HWLoop must be aligned
+** HWLoop body must contain at least 3 instructions
+** No compressed instructions allowed in the HWLoop body
+** The End address of the outermost HWLoop (#1) must be at least 2 instructions further thatn the End address innermost HWloop (#0), i.e. HWLoop[1].endaddress &gt;= HWLoop[0].endaddress + 8
+** Last instruction cannot be any jump or branch instruction</t>
+  </si>
+  <si>
+    <t>RI5CY: User Manual, rev. 4.3
+Section 7</t>
+  </si>
+  <si>
+    <t>RI5CY: User Manual, rev. 4.3
+Section 14.2</t>
+  </si>
+  <si>
+    <t>Hardware loop</t>
   </si>
 </sst>
 </file>
@@ -802,11 +788,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMK12"/>
+  <dimension ref="A1:AMK11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
+      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -814,7 +800,7 @@
     <col min="1" max="1" width="32.77734375" style="1" customWidth="1"/>
     <col min="2" max="2" width="28" style="1" customWidth="1"/>
     <col min="3" max="3" width="22.44140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="51.21875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="55.33203125" style="1" customWidth="1"/>
     <col min="5" max="5" width="51" style="1" customWidth="1"/>
     <col min="6" max="6" width="34.5546875" style="1" customWidth="1"/>
     <col min="7" max="7" width="12.33203125" style="1" customWidth="1"/>
@@ -855,28 +841,28 @@
     </row>
     <row r="2" spans="1:9" s="4" customFormat="1" ht="55.2">
       <c r="A2" s="18" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C2" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>31</v>
-      </c>
       <c r="G2" s="8" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="I2" s="6"/>
     </row>
@@ -884,91 +870,91 @@
       <c r="A3" s="18"/>
       <c r="B3" s="19"/>
       <c r="C3" s="8" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="I3" s="6"/>
     </row>
-    <row r="4" spans="1:9" s="4" customFormat="1" ht="138">
+    <row r="4" spans="1:9" s="4" customFormat="1" ht="184.8" customHeight="1">
       <c r="A4" s="18"/>
       <c r="B4" s="19"/>
-      <c r="C4" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="G4" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="H4" s="10" t="s">
-        <v>38</v>
-      </c>
+      <c r="C4" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" s="13"/>
+      <c r="H4" s="14"/>
       <c r="I4" s="6"/>
     </row>
-    <row r="5" spans="1:9" s="4" customFormat="1" ht="184.8" customHeight="1">
-      <c r="A5" s="18"/>
-      <c r="B5" s="19"/>
-      <c r="C5" s="11" t="s">
+    <row r="5" spans="1:9" s="4" customFormat="1" ht="28.2">
+      <c r="A5" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="F5" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="G5" s="13"/>
-      <c r="H5" s="14"/>
+      <c r="F5" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>28</v>
+      </c>
       <c r="I5" s="6"/>
     </row>
     <row r="6" spans="1:9" s="4" customFormat="1" ht="28.2">
-      <c r="A6" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="18" t="s">
-        <v>13</v>
-      </c>
+      <c r="A6" s="18"/>
+      <c r="B6" s="18"/>
       <c r="C6" s="7" t="s">
         <v>12</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="I6" s="6"/>
     </row>
@@ -976,22 +962,22 @@
       <c r="A7" s="18"/>
       <c r="B7" s="18"/>
       <c r="C7" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="I7" s="6"/>
     </row>
@@ -999,114 +985,91 @@
       <c r="A8" s="18"/>
       <c r="B8" s="18"/>
       <c r="C8" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="I8" s="6"/>
     </row>
-    <row r="9" spans="1:9" s="4" customFormat="1" ht="28.2">
+    <row r="9" spans="1:9" s="5" customFormat="1" ht="55.8">
       <c r="A9" s="18"/>
       <c r="B9" s="18"/>
       <c r="C9" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="H9" s="9" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="I9" s="6"/>
     </row>
-    <row r="10" spans="1:9" s="5" customFormat="1" ht="55.8">
+    <row r="10" spans="1:9" ht="55.8">
       <c r="A10" s="18"/>
       <c r="B10" s="18"/>
       <c r="C10" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="7" t="s">
-        <v>20</v>
-      </c>
       <c r="E10" s="15" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="I10" s="6"/>
     </row>
-    <row r="11" spans="1:9" ht="55.8">
-      <c r="A11" s="18"/>
-      <c r="B11" s="18"/>
-      <c r="C11" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E11" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="H11" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="I11" s="6"/>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12" s="17" t="s">
+    <row r="11" spans="1:9">
+      <c r="A11" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="17"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="17"/>
-      <c r="I12" s="17"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="A12:I12"/>
-    <mergeCell ref="A6:A11"/>
-    <mergeCell ref="B6:B11"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="A11:I11"/>
+    <mergeCell ref="A5:A10"/>
+    <mergeCell ref="B5:B10"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="B2:B4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>